<commit_message>
Ajout tâche réalisée dans tableau de bord
</commit_message>
<xml_diff>
--- a/Tableau de bord.xlsx
+++ b/Tableau de bord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PHP\Projet\projectPHP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B967AB-7BE3-469A-9389-6DBC971294D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52544C2-EE7B-4FC3-AD57-2B6CF56DDADE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2265" windowWidth="21600" windowHeight="11385" xr2:uid="{0269BC55-9499-4618-8092-600EE3F0C448}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Nom</t>
   </si>
@@ -47,15 +47,29 @@
   <si>
     <t>Contribution</t>
   </si>
+  <si>
+    <t>François</t>
+  </si>
+  <si>
+    <t>Création du tableau de bord</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,14 +95,93 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF00FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -397,25 +490,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35555EA8-B618-43E7-B075-D8312B4E157D}">
-  <dimension ref="B2:E2"/>
+  <dimension ref="B2:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
@@ -425,7 +518,33 @@
         <v>3</v>
       </c>
     </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="3">
+        <v>44183</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>"François"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"Anthony"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>"Thomas"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Lucas"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout dans tableau de bord
</commit_message>
<xml_diff>
--- a/Tableau de bord.xlsx
+++ b/Tableau de bord.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PHP\Projet\projectPHP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Xampp\htdocs\ANTHONY\projectPHP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52544C2-EE7B-4FC3-AD57-2B6CF56DDADE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C334096B-0022-42FC-9AE0-5C8DE8251FB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2265" windowWidth="21600" windowHeight="11385" xr2:uid="{0269BC55-9499-4618-8092-600EE3F0C448}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0269BC55-9499-4618-8092-600EE3F0C448}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Nom</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Création du tableau de bord</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>Partie 1</t>
   </si>
 </sst>
 </file>
@@ -104,46 +110,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF00FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -158,13 +129,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -490,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35555EA8-B618-43E7-B075-D8312B4E157D}">
-  <dimension ref="B2:E10"/>
+  <dimension ref="B2:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,18 +493,32 @@
         <v>5</v>
       </c>
     </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <v>44183</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"François"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Anthony"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Thomas"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Lucas"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Ajout création de liste
</commit_message>
<xml_diff>
--- a/Tableau de bord.xlsx
+++ b/Tableau de bord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Xampp\htdocs\ANTHONY\projectPHP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C334096B-0022-42FC-9AE0-5C8DE8251FB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638BAA9D-645D-428B-8E68-D7C854958CB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0269BC55-9499-4618-8092-600EE3F0C448}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Nom</t>
   </si>
@@ -57,7 +57,10 @@
     <t>Anthony</t>
   </si>
   <si>
-    <t>Partie 1</t>
+    <t>N°1</t>
+  </si>
+  <si>
+    <t>Tout</t>
   </si>
 </sst>
 </file>
@@ -454,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35555EA8-B618-43E7-B075-D8312B4E157D}">
-  <dimension ref="B2:E11"/>
+  <dimension ref="B2:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,6 +507,20 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>44185</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Affichage des listes public
</commit_message>
<xml_diff>
--- a/Tableau de bord.xlsx
+++ b/Tableau de bord.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PHP\Projet\projectPHP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Xampp\htdocs\ANTHONY\projectPHP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE93399-671F-449C-AC7F-937B522708E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC8BFD7-7576-4920-B165-937AC7BC2DC0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0269BC55-9499-4618-8092-600EE3F0C448}"/>
+    <workbookView xWindow="3840" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{0269BC55-9499-4618-8092-600EE3F0C448}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>Nom</t>
   </si>
@@ -125,7 +125,91 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -469,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35555EA8-B618-43E7-B075-D8312B4E157D}">
-  <dimension ref="B2:E10"/>
+  <dimension ref="B2:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,7 +617,7 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -606,8 +690,36 @@
         <v>12</v>
       </c>
     </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <v>44204</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C17:C1048576 C1:C10">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+      <formula>"Lucas"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+      <formula>"Thomas"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+      <formula>"Anthony"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+      <formula>"François"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Lucas"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Maj Tableau de bord
</commit_message>
<xml_diff>
--- a/Tableau de bord.xlsx
+++ b/Tableau de bord.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PHP\Projet\projectPHP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Xampp\htdocs\ANTHONY\projectPHP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E64B60-EAA9-48C3-98A2-608DCA75CD15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314C6E52-07B5-441F-8942-3F8E14154990}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0269BC55-9499-4618-8092-600EE3F0C448}"/>
+    <workbookView xWindow="3840" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{0269BC55-9499-4618-8092-600EE3F0C448}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>Nom</t>
   </si>
@@ -81,6 +81,9 @@
   <si>
     <t>Tout
 Tout</t>
+  </si>
+  <si>
+    <t>Affichage et titre clicable</t>
   </si>
 </sst>
 </file>
@@ -136,7 +139,91 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -564,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35555EA8-B618-43E7-B075-D8312B4E157D}">
-  <dimension ref="B2:E13"/>
+  <dimension ref="B2:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,36 +830,92 @@
         <v>14</v>
       </c>
     </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <v>44205</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
+        <v>44205</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C17:C1048576 C1:C10">
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="21" operator="equal">
       <formula>"Lucas"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
       <formula>"Thomas"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="23" operator="equal">
       <formula>"Anthony"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
       <formula>"François"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
       <formula>"Lucas"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="18" operator="equal">
       <formula>"Thomas"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
       <formula>"Anthony"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
       <formula>"François"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
+    <cfRule type="cellIs" dxfId="19" priority="13" operator="equal">
+      <formula>"Lucas"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
+      <formula>"Thomas"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
+      <formula>"Anthony"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
+      <formula>"François"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+      <formula>"Lucas"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+      <formula>"Thomas"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+      <formula>"Anthony"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+      <formula>"François"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
     <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"Lucas"</formula>
     </cfRule>
@@ -786,7 +929,7 @@
       <formula>"François"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
+  <conditionalFormatting sqref="C15">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Lucas"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Finitions pour affichages des listes
</commit_message>
<xml_diff>
--- a/Tableau de bord.xlsx
+++ b/Tableau de bord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Xampp\htdocs\ANTHONY\projectPHP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314C6E52-07B5-441F-8942-3F8E14154990}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300DE598-B53F-4B5C-A059-32EB0A3E4BFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{0269BC55-9499-4618-8092-600EE3F0C448}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
   <si>
     <t>Nom</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Affichage et titre clicable</t>
+  </si>
+  <si>
+    <t>Fini</t>
   </si>
 </sst>
 </file>
@@ -651,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35555EA8-B618-43E7-B075-D8312B4E157D}">
-  <dimension ref="B2:E15"/>
+  <dimension ref="B2:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,64 +861,92 @@
         <v>15</v>
       </c>
     </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="3">
+        <v>44206</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>21</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C17:C1048576 C1:C10">
-    <cfRule type="cellIs" dxfId="27" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
       <formula>"Lucas"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
       <formula>"Thomas"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
       <formula>"Anthony"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
       <formula>"François"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
       <formula>"Lucas"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
       <formula>"Thomas"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
       <formula>"Anthony"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
       <formula>"François"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="cellIs" dxfId="19" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
       <formula>"Lucas"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
       <formula>"Thomas"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
       <formula>"Anthony"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
       <formula>"François"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"Lucas"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
       <formula>"Thomas"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
       <formula>"Anthony"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
       <formula>"François"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+      <formula>"Lucas"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+      <formula>"Thomas"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+      <formula>"Anthony"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+      <formula>"François"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
     <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"Lucas"</formula>
     </cfRule>
@@ -929,7 +960,7 @@
       <formula>"François"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
+  <conditionalFormatting sqref="C16">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Lucas"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Ajout d'une liste sur un compte avec un token
</commit_message>
<xml_diff>
--- a/Tableau de bord.xlsx
+++ b/Tableau de bord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\XAMPP\htdocs\php\projet\projectPHP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77867910-FD0B-489A-B46B-0255D9101A46}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6919F6CF-A188-4BAE-840A-2C2B037FA1B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{0269BC55-9499-4618-8092-600EE3F0C448}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
   <si>
     <t>Nom</t>
   </si>
@@ -98,10 +98,12 @@
   <si>
     <t>11
 12
-13</t>
+13
+28</t>
   </si>
   <si>
     <t>Tout
+Tout
 Tout
 Tout</t>
   </si>
@@ -159,7 +161,35 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="40">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -727,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35555EA8-B618-43E7-B075-D8312B4E157D}">
-  <dimension ref="B2:E19"/>
+  <dimension ref="B2:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,15 +958,15 @@
         <v>6</v>
       </c>
       <c r="D15">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
-        <v>44206</v>
+        <v>44205</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>6</v>
@@ -945,7 +975,7 @@
         <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -956,42 +986,70 @@
         <v>6</v>
       </c>
       <c r="D17">
+        <v>21</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
+        <v>44206</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18">
         <v>8</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="3">
-        <v>44208</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <v>44208</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B20" s="3">
+        <v>44208</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C19:C1048576 C1:C10">
+  <conditionalFormatting sqref="C1:C10 C20:C1048576">
+    <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
+      <formula>"Lucas"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="38" operator="equal">
+      <formula>"Thomas"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="39" operator="equal">
+      <formula>"Anthony"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="40" operator="equal">
+      <formula>"François"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
     <cfRule type="cellIs" dxfId="35" priority="33" operator="equal">
       <formula>"Lucas"</formula>
     </cfRule>
@@ -1005,7 +1063,7 @@
       <formula>"François"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
+  <conditionalFormatting sqref="C11">
     <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
       <formula>"Lucas"</formula>
     </cfRule>
@@ -1019,7 +1077,7 @@
       <formula>"François"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11">
+  <conditionalFormatting sqref="C13">
     <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
       <formula>"Lucas"</formula>
     </cfRule>
@@ -1033,7 +1091,7 @@
       <formula>"François"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
+  <conditionalFormatting sqref="C14">
     <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
       <formula>"Lucas"</formula>
     </cfRule>
@@ -1047,7 +1105,7 @@
       <formula>"François"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
+  <conditionalFormatting sqref="C16">
     <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
       <formula>"Lucas"</formula>
     </cfRule>
@@ -1061,7 +1119,7 @@
       <formula>"François"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
+  <conditionalFormatting sqref="C17">
     <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"Lucas"</formula>
     </cfRule>
@@ -1075,7 +1133,7 @@
       <formula>"François"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C16">
+  <conditionalFormatting sqref="C18">
     <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"Lucas"</formula>
     </cfRule>
@@ -1089,7 +1147,7 @@
       <formula>"François"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
+  <conditionalFormatting sqref="C19">
     <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"Lucas"</formula>
     </cfRule>
@@ -1103,7 +1161,7 @@
       <formula>"François"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
+  <conditionalFormatting sqref="C15">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Lucas"</formula>
     </cfRule>

</xml_diff>